<commit_message>
adding 'Screenshot' method nad ITestListerner
</commit_message>
<xml_diff>
--- a/AutomationDemo/src/test/resources/testdata/automation_testdata.xlsx
+++ b/AutomationDemo/src/test/resources/testdata/automation_testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="343">
   <si>
     <t>username</t>
   </si>
@@ -1050,6 +1050,9 @@
   </si>
   <si>
     <t>09231993</t>
+  </si>
+  <si>
+    <t>07081992</t>
   </si>
 </sst>
 </file>
@@ -2452,7 +2455,7 @@
         <v>320</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2460,7 +2463,7 @@
         <v>321</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2468,7 +2471,7 @@
         <v>322</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>